<commit_message>
all the updates to the code
</commit_message>
<xml_diff>
--- a/04_Data/open_responses/English FINISHED/psa004_OEQ_JM_ENG FINISHED.xlsx
+++ b/04_Data/open_responses/English FINISHED/psa004_OEQ_JM_ENG FINISHED.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="768">
   <si>
     <t xml:space="preserve">Thank you for volunteering to help with the open-ended response coding for PSA 004. </t>
   </si>
@@ -137,6 +137,9 @@
     <t xml:space="preserve">To see the perception of the people participating in the study on whether or not another person's perception is believable or not. </t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>s621</t>
   </si>
   <si>
@@ -750,9 +753,6 @@
     <t>To determine how {Category:} think differently of believing and knowing.</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>s1122</t>
   </si>
   <si>
@@ -2128,6 +2128,9 @@
   </si>
   <si>
     <t>I think the purpose of this study was to determine how people assume they perceive the world when in actuality they may be perceiving incorrectly</t>
+  </si>
+  <si>
+    <t>maybe</t>
   </si>
   <si>
     <t>s2910</t>
@@ -2407,7 +2410,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2425,6 +2428,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -4347,17 +4353,19 @@
       <c r="C13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
@@ -4365,13 +4373,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>10</v>
@@ -4379,13 +4387,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>17</v>
@@ -4393,13 +4401,13 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>10</v>
@@ -4407,13 +4415,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>10</v>
@@ -4421,13 +4429,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>17</v>
@@ -4435,13 +4443,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>10</v>
@@ -4449,13 +4457,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>10</v>
@@ -4463,13 +4471,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>10</v>
@@ -4477,27 +4485,27 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>10</v>
@@ -4505,13 +4513,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>10</v>
@@ -4519,13 +4527,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>17</v>
@@ -4533,13 +4541,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>10</v>
@@ -4547,13 +4555,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>10</v>
@@ -4561,13 +4569,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>10</v>
@@ -4575,13 +4583,13 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>17</v>
@@ -4589,13 +4597,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>10</v>
@@ -4603,13 +4611,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>10</v>
@@ -4617,13 +4625,13 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>10</v>
@@ -4631,13 +4639,13 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>10</v>
@@ -4645,13 +4653,13 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>10</v>
@@ -4659,13 +4667,13 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>10</v>
@@ -4673,13 +4681,13 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>10</v>
@@ -4687,13 +4695,13 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>10</v>
@@ -4701,13 +4709,13 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>10</v>
@@ -4715,13 +4723,13 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>10</v>
@@ -4729,13 +4737,13 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>10</v>
@@ -4743,13 +4751,13 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>17</v>
@@ -4757,13 +4765,13 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>10</v>
@@ -4771,13 +4779,13 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>10</v>
@@ -4785,13 +4793,13 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>10</v>
@@ -4799,13 +4807,13 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>10</v>
@@ -4813,13 +4821,13 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>10</v>
@@ -4827,13 +4835,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>10</v>
@@ -4841,13 +4849,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>17</v>
@@ -4855,13 +4863,13 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>17</v>
@@ -4869,13 +4877,13 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>10</v>
@@ -4883,13 +4891,13 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>10</v>
@@ -4897,13 +4905,13 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>17</v>
@@ -4911,13 +4919,13 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>10</v>
@@ -4925,13 +4933,13 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>10</v>
@@ -4939,13 +4947,13 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>10</v>
@@ -4953,13 +4961,13 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>10</v>
@@ -4967,13 +4975,13 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>10</v>
@@ -4981,27 +4989,27 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>10</v>
@@ -5009,13 +5017,13 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>10</v>
@@ -5023,13 +5031,13 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>10</v>
@@ -5037,13 +5045,13 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>10</v>
@@ -5051,41 +5059,41 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="D65" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>10</v>
@@ -5093,13 +5101,13 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>10</v>
@@ -5107,13 +5115,13 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>10</v>
@@ -5121,13 +5129,13 @@
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>10</v>
@@ -5135,13 +5143,13 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>10</v>
@@ -5149,13 +5157,13 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>17</v>
@@ -5163,13 +5171,13 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>10</v>
@@ -5177,13 +5185,13 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>10</v>
@@ -5191,13 +5199,13 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>10</v>
@@ -5205,13 +5213,13 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>17</v>
@@ -5219,13 +5227,13 @@
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>10</v>
@@ -5233,13 +5241,13 @@
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>10</v>
@@ -5247,13 +5255,13 @@
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>10</v>
@@ -5261,13 +5269,13 @@
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>10</v>
@@ -5275,13 +5283,13 @@
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>10</v>
@@ -5289,13 +5297,13 @@
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>10</v>
@@ -5303,13 +5311,13 @@
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>10</v>
@@ -5317,13 +5325,13 @@
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>10</v>
@@ -5331,13 +5339,13 @@
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>10</v>
@@ -5345,27 +5353,27 @@
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>10</v>
@@ -5373,13 +5381,13 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>10</v>
@@ -5387,13 +5395,13 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>17</v>
@@ -5401,13 +5409,13 @@
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>10</v>
@@ -5415,13 +5423,13 @@
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>10</v>
@@ -5429,13 +5437,13 @@
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>10</v>
@@ -5443,13 +5451,13 @@
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>10</v>
@@ -5457,13 +5465,13 @@
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>10</v>
@@ -5471,13 +5479,13 @@
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>10</v>
@@ -5485,13 +5493,13 @@
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>10</v>
@@ -5499,13 +5507,13 @@
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>10</v>
@@ -5513,13 +5521,13 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>10</v>
@@ -5527,13 +5535,13 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>10</v>
@@ -5541,13 +5549,13 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>10</v>
@@ -5555,13 +5563,13 @@
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>10</v>
@@ -5569,13 +5577,13 @@
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>10</v>
@@ -5583,13 +5591,13 @@
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>10</v>
@@ -5597,13 +5605,13 @@
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>10</v>
@@ -5611,13 +5619,13 @@
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>10</v>
@@ -5625,13 +5633,13 @@
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>10</v>
@@ -5639,13 +5647,13 @@
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>10</v>
@@ -5653,13 +5661,13 @@
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>10</v>
@@ -5667,13 +5675,13 @@
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>17</v>
@@ -5681,13 +5689,13 @@
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>10</v>
@@ -5695,13 +5703,13 @@
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>10</v>
@@ -5709,13 +5717,13 @@
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>10</v>
@@ -5723,13 +5731,13 @@
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>10</v>
@@ -5737,27 +5745,27 @@
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>17</v>
@@ -5765,44 +5773,44 @@
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>238</v>
+        <v>34</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
@@ -5813,10 +5821,10 @@
         <v>8</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>238</v>
+        <v>34</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
@@ -5830,7 +5838,7 @@
         <v>241</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>238</v>
+        <v>34</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
@@ -5841,10 +5849,10 @@
         <v>8</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>238</v>
+        <v>34</v>
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1">
@@ -5855,10 +5863,10 @@
         <v>8</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>238</v>
+        <v>34</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
@@ -5869,10 +5877,10 @@
         <v>8</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
@@ -5883,10 +5891,10 @@
         <v>8</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
@@ -5897,10 +5905,10 @@
         <v>8</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
@@ -5911,10 +5919,10 @@
         <v>8</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
@@ -5925,10 +5933,10 @@
         <v>8</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
@@ -6429,10 +6437,10 @@
         <v>8</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="163" ht="15.75" customHeight="1">
@@ -6443,10 +6451,10 @@
         <v>8</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="164" ht="15.75" customHeight="1">
@@ -6457,10 +6465,10 @@
         <v>8</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="165" ht="15.75" customHeight="1">
@@ -6471,10 +6479,10 @@
         <v>8</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="166" ht="15.75" customHeight="1">
@@ -6569,7 +6577,7 @@
         <v>8</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D172" s="4" t="s">
         <v>10</v>
@@ -6681,10 +6689,10 @@
         <v>8</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D180" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="181" ht="15.75" customHeight="1">
@@ -6695,10 +6703,10 @@
         <v>8</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D181" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="182" ht="15.75" customHeight="1">
@@ -6723,10 +6731,10 @@
         <v>8</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="184" ht="15.75" customHeight="1">
@@ -7143,10 +7151,10 @@
         <v>8</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D213" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="214" ht="15.75" customHeight="1">
@@ -7157,10 +7165,10 @@
         <v>8</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D214" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="215" ht="15.75" customHeight="1">
@@ -7171,10 +7179,10 @@
         <v>8</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D215" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="216" ht="15.75" customHeight="1">
@@ -7185,10 +7193,10 @@
         <v>8</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="217" ht="15.75" customHeight="1">
@@ -7199,10 +7207,10 @@
         <v>8</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D217" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="218" ht="15.75" customHeight="1">
@@ -7213,10 +7221,10 @@
         <v>8</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="219" ht="15.75" customHeight="1">
@@ -7255,10 +7263,10 @@
         <v>8</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="222" ht="15.75" customHeight="1">
@@ -7479,10 +7487,10 @@
         <v>8</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D237" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="238" ht="15.75" customHeight="1">
@@ -7941,10 +7949,10 @@
         <v>8</v>
       </c>
       <c r="C270" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D270" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="271" ht="15.75" customHeight="1">
@@ -8125,7 +8133,9 @@
       <c r="C283" s="3" t="s">
         <v>541</v>
       </c>
-      <c r="D283" s="4"/>
+      <c r="D283" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="284" ht="15.75" customHeight="1">
       <c r="A284" s="4" t="s">
@@ -8389,7 +8399,9 @@
       <c r="C302" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="D302" s="4"/>
+      <c r="D302" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="303" ht="15.75" customHeight="1">
       <c r="A303" s="4" t="s">
@@ -8511,10 +8523,10 @@
         <v>8</v>
       </c>
       <c r="C311" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D311" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="312" ht="15.75" customHeight="1">
@@ -8695,7 +8707,9 @@
       <c r="C324" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="D324" s="4"/>
+      <c r="D324" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="325" ht="15.75" customHeight="1">
       <c r="A325" s="4" t="s">
@@ -8747,10 +8761,10 @@
         <v>8</v>
       </c>
       <c r="C328" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D328" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="329" ht="15.75" customHeight="1">
@@ -8761,10 +8775,10 @@
         <v>8</v>
       </c>
       <c r="C329" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D329" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="330" ht="15.75" customHeight="1">
@@ -8775,10 +8789,10 @@
         <v>8</v>
       </c>
       <c r="C330" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D330" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="331" ht="15.75" customHeight="1">
@@ -8789,10 +8803,10 @@
         <v>8</v>
       </c>
       <c r="C331" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D331" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="332" ht="15.75" customHeight="1">
@@ -8806,7 +8820,7 @@
         <v>634</v>
       </c>
       <c r="D332" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="333" ht="15.75" customHeight="1">
@@ -9055,7 +9069,7 @@
         <v>8</v>
       </c>
       <c r="C350" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D350" s="4" t="s">
         <v>10</v>
@@ -9083,10 +9097,10 @@
         <v>8</v>
       </c>
       <c r="C352" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D352" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="353" ht="15.75" customHeight="1">
@@ -9181,7 +9195,7 @@
         <v>8</v>
       </c>
       <c r="C359" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D359" s="4" t="s">
         <v>10</v>
@@ -9281,17 +9295,19 @@
       <c r="C366" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="D366" s="4"/>
+      <c r="D366" s="8" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="367" ht="15.75" customHeight="1">
       <c r="A367" s="4" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B367" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C367" s="3" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D367" s="4" t="s">
         <v>17</v>
@@ -9299,13 +9315,13 @@
     </row>
     <row r="368" ht="15.75" customHeight="1">
       <c r="A368" s="4" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B368" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C368" s="3" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="D368" s="4" t="s">
         <v>17</v>
@@ -9313,13 +9329,13 @@
     </row>
     <row r="369" ht="15.75" customHeight="1">
       <c r="A369" s="4" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B369" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C369" s="3" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D369" s="4" t="s">
         <v>17</v>
@@ -9327,13 +9343,13 @@
     </row>
     <row r="370" ht="15.75" customHeight="1">
       <c r="A370" s="4" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B370" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C370" s="3" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D370" s="4" t="s">
         <v>17</v>
@@ -9341,13 +9357,13 @@
     </row>
     <row r="371" ht="15.75" customHeight="1">
       <c r="A371" s="4" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B371" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C371" s="3" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="D371" s="4" t="s">
         <v>10</v>
@@ -9355,13 +9371,13 @@
     </row>
     <row r="372" ht="15.75" customHeight="1">
       <c r="A372" s="4" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B372" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C372" s="3" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="D372" s="4" t="s">
         <v>10</v>
@@ -9369,13 +9385,13 @@
     </row>
     <row r="373" ht="15.75" customHeight="1">
       <c r="A373" s="4" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B373" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C373" s="3" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="D373" s="4" t="s">
         <v>17</v>
@@ -9383,13 +9399,13 @@
     </row>
     <row r="374" ht="15.75" customHeight="1">
       <c r="A374" s="4" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B374" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C374" s="3" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D374" s="4" t="s">
         <v>10</v>
@@ -9397,13 +9413,13 @@
     </row>
     <row r="375" ht="15.75" customHeight="1">
       <c r="A375" s="4" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B375" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C375" s="3" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D375" s="4" t="s">
         <v>10</v>
@@ -9411,27 +9427,27 @@
     </row>
     <row r="376" ht="15.75" customHeight="1">
       <c r="A376" s="4" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B376" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C376" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D376" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="377" ht="15.75" customHeight="1">
       <c r="A377" s="4" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B377" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C377" s="3" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="D377" s="4" t="s">
         <v>10</v>
@@ -9439,13 +9455,13 @@
     </row>
     <row r="378" ht="15.75" customHeight="1">
       <c r="A378" s="4" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B378" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C378" s="3" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="D378" s="4" t="s">
         <v>10</v>
@@ -9453,13 +9469,13 @@
     </row>
     <row r="379" ht="15.75" customHeight="1">
       <c r="A379" s="4" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B379" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C379" s="3" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D379" s="4" t="s">
         <v>10</v>
@@ -9467,13 +9483,13 @@
     </row>
     <row r="380" ht="15.75" customHeight="1">
       <c r="A380" s="4" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B380" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C380" s="3" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="D380" s="4" t="s">
         <v>10</v>
@@ -9481,13 +9497,13 @@
     </row>
     <row r="381" ht="15.75" customHeight="1">
       <c r="A381" s="4" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B381" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C381" s="3" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="D381" s="4" t="s">
         <v>10</v>
@@ -9495,13 +9511,13 @@
     </row>
     <row r="382" ht="15.75" customHeight="1">
       <c r="A382" s="4" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B382" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C382" s="3" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="D382" s="4" t="s">
         <v>10</v>
@@ -9509,13 +9525,13 @@
     </row>
     <row r="383" ht="15.75" customHeight="1">
       <c r="A383" s="4" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B383" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C383" s="3" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D383" s="4" t="s">
         <v>10</v>
@@ -9523,13 +9539,13 @@
     </row>
     <row r="384" ht="15.75" customHeight="1">
       <c r="A384" s="4" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B384" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C384" s="3" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="D384" s="4" t="s">
         <v>10</v>
@@ -9537,13 +9553,13 @@
     </row>
     <row r="385" ht="15.75" customHeight="1">
       <c r="A385" s="4" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B385" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C385" s="3" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="D385" s="4" t="s">
         <v>10</v>
@@ -9551,13 +9567,13 @@
     </row>
     <row r="386" ht="15.75" customHeight="1">
       <c r="A386" s="4" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B386" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C386" s="3" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D386" s="4" t="s">
         <v>10</v>
@@ -9565,13 +9581,13 @@
     </row>
     <row r="387" ht="15.75" customHeight="1">
       <c r="A387" s="4" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B387" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C387" s="3" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="D387" s="4" t="s">
         <v>10</v>
@@ -9579,13 +9595,13 @@
     </row>
     <row r="388" ht="15.75" customHeight="1">
       <c r="A388" s="4" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B388" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C388" s="3" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D388" s="4" t="s">
         <v>10</v>
@@ -9593,13 +9609,13 @@
     </row>
     <row r="389" ht="15.75" customHeight="1">
       <c r="A389" s="4" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B389" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C389" s="3" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="D389" s="4" t="s">
         <v>10</v>
@@ -9607,13 +9623,13 @@
     </row>
     <row r="390" ht="15.75" customHeight="1">
       <c r="A390" s="4" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B390" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C390" s="3" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="D390" s="4" t="s">
         <v>10</v>
@@ -9621,13 +9637,13 @@
     </row>
     <row r="391" ht="15.75" customHeight="1">
       <c r="A391" s="4" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B391" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C391" s="3" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="D391" s="4" t="s">
         <v>17</v>
@@ -9635,13 +9651,13 @@
     </row>
     <row r="392" ht="15.75" customHeight="1">
       <c r="A392" s="4" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B392" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C392" s="3" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D392" s="4" t="s">
         <v>10</v>
@@ -9649,13 +9665,13 @@
     </row>
     <row r="393" ht="15.75" customHeight="1">
       <c r="A393" s="4" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B393" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C393" s="3" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="D393" s="4" t="s">
         <v>10</v>
@@ -9663,13 +9679,13 @@
     </row>
     <row r="394" ht="15.75" customHeight="1">
       <c r="A394" s="4" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B394" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C394" s="3" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="D394" s="4" t="s">
         <v>10</v>
@@ -9677,13 +9693,13 @@
     </row>
     <row r="395" ht="15.75" customHeight="1">
       <c r="A395" s="4" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B395" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C395" s="3" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="D395" s="4" t="s">
         <v>10</v>
@@ -9691,13 +9707,13 @@
     </row>
     <row r="396" ht="15.75" customHeight="1">
       <c r="A396" s="4" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B396" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C396" s="3" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="D396" s="4" t="s">
         <v>10</v>
@@ -9705,13 +9721,13 @@
     </row>
     <row r="397" ht="15.75" customHeight="1">
       <c r="A397" s="4" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B397" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C397" s="3" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D397" s="4" t="s">
         <v>10</v>
@@ -9719,13 +9735,13 @@
     </row>
     <row r="398" ht="15.75" customHeight="1">
       <c r="A398" s="4" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B398" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C398" s="3" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="D398" s="4" t="s">
         <v>17</v>
@@ -9733,13 +9749,13 @@
     </row>
     <row r="399" ht="15.75" customHeight="1">
       <c r="A399" s="4" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B399" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C399" s="3" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="D399" s="4" t="s">
         <v>10</v>
@@ -9747,29 +9763,29 @@
     </row>
     <row r="400" ht="15.75" customHeight="1">
       <c r="A400" s="4" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B400" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C400" s="3" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D400" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="401" ht="15.75" customHeight="1">
-      <c r="A401" s="8" t="s">
-        <v>765</v>
-      </c>
-      <c r="B401" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C401" s="8" t="s">
+      <c r="A401" s="9" t="s">
         <v>766</v>
       </c>
-      <c r="D401" s="9" t="s">
+      <c r="B401" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C401" s="9" t="s">
+        <v>767</v>
+      </c>
+      <c r="D401" s="10" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>